<commit_message>
Adding NCI60 kmeans, clara results in excel
</commit_message>
<xml_diff>
--- a/notebooks/local/sensitivity_cer.xlsx
+++ b/notebooks/local/sensitivity_cer.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neo\workspace-r\evaluomeR\notebooks\local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E2C3DF-498C-4189-8D78-5070E8672EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E2F992-5EB8-468E-95F7-80A80F6AF29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{84853FC6-BCE5-4519-99D7-EACBF2F3B783}"/>
   </bookViews>
   <sheets>
     <sheet name="NCI60 - 10 cat - kmeans" sheetId="3" r:id="rId1"/>
     <sheet name="NCI60 - 8 cat - kmeans" sheetId="5" r:id="rId2"/>
-    <sheet name="NCI60 - 8 cat - clara" sheetId="7" r:id="rId3"/>
+    <sheet name="NCI60 - 10 cat - clara" sheetId="7" r:id="rId3"/>
+    <sheet name="NCI60 - 8 cat - clara" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
   <si>
     <t>Optimal K</t>
   </si>
@@ -272,6 +273,55 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
+      <xdr:colOff>715432</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>182011</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368549FD-1C1B-9681-DD68-DD4EBBC3FBE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7573432" cy="7421011"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>724958</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>134379</xdr:rowOff>
@@ -281,7 +331,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B58C52D-F1A7-4045-BF5D-2B9B9DE6F8A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E87249A-7906-40B4-B7DA-52A0ED962CBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -786,6 +836,84 @@
   <dimension ref="K7:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.68775315656565705</v>
+      </c>
+    </row>
+    <row r="11" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.156800514534358</v>
+      </c>
+    </row>
+    <row r="12" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.13489999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25F2666-4DFC-4061-822C-68D630984F1C}">
+  <dimension ref="K7:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding excel data for CER and Sensitivity for Golub
</commit_message>
<xml_diff>
--- a/notebooks/local/sensitivity_cer.xlsx
+++ b/notebooks/local/sensitivity_cer.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neo\workspace-r\evaluomeR\notebooks\local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E2F992-5EB8-468E-95F7-80A80F6AF29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707A0562-6C9B-4988-8B00-7A88067C9916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{84853FC6-BCE5-4519-99D7-EACBF2F3B783}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{84853FC6-BCE5-4519-99D7-EACBF2F3B783}"/>
   </bookViews>
   <sheets>
     <sheet name="NCI60 - 10 cat - kmeans" sheetId="3" r:id="rId1"/>
     <sheet name="NCI60 - 8 cat - kmeans" sheetId="5" r:id="rId2"/>
     <sheet name="NCI60 - 10 cat - clara" sheetId="7" r:id="rId3"/>
     <sheet name="NCI60 - 8 cat - clara" sheetId="8" r:id="rId4"/>
+    <sheet name="Golub - 3 cat - kmeans" sheetId="10" r:id="rId5"/>
+    <sheet name="Golub - 3 cat - clara" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
   <si>
     <t>Optimal K</t>
   </si>
@@ -324,14 +326,14 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>724958</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>134379</xdr:rowOff>
+      <xdr:rowOff>124853</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E87249A-7906-40B4-B7DA-52A0ED962CBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46868C4D-21B3-D242-4A3E-0C5277841401}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -348,7 +350,105 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7582958" cy="7373379"/>
+          <a:ext cx="7582958" cy="7363853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10590</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>48642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28AAC699-9D12-B587-56B5-C25FB946D434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7630590" cy="7287642"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>705906</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>58168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B61CCA56-F5F2-88C2-2C57-9DA36A342A56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7563906" cy="7297168"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,10 +777,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F089715D-DE43-49C5-BE92-166D83C453D7}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="K7:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0B3587-C4D9-43D1-B927-08A2EDF5B9A3}">
   <dimension ref="K7:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -914,7 +1017,7 @@
   <dimension ref="K7:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="11:14" x14ac:dyDescent="0.25">
@@ -951,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="5">
-        <v>0</v>
+        <v>0.75609158813609301</v>
       </c>
     </row>
     <row r="11" spans="11:14" x14ac:dyDescent="0.25">
@@ -959,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="L11" s="5">
-        <v>0</v>
+        <v>0.14423391846252501</v>
       </c>
     </row>
     <row r="12" spans="11:14" x14ac:dyDescent="0.25">
@@ -967,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="L12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="11:14" x14ac:dyDescent="0.25">
@@ -975,7 +1078,166 @@
         <v>5</v>
       </c>
       <c r="L13" s="3">
+        <v>0.1492</v>
+      </c>
+    </row>
+    <row r="15" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF133B14-376C-4A84-B6FF-AECFC4834039}">
+  <dimension ref="K7:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.67624415193500298</v>
+      </c>
+    </row>
+    <row r="11" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.189987264023665</v>
+      </c>
+    </row>
+    <row r="12" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="13" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>7.4300000000000005E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC0E12A-CF84-42ED-847A-10D1C66235F4}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="K7:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.78530918036428998</v>
+      </c>
+    </row>
+    <row r="11" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.23201412622581999</v>
+      </c>
+    </row>
+    <row r="12" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.97370000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>3.7600000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="11:14" x14ac:dyDescent="0.25">

</xml_diff>